<commit_message>
ajout de formule + format cell
</commit_message>
<xml_diff>
--- a/excel/statFacture3.xlsx
+++ b/excel/statFacture3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>statistique des factures</t>
   </si>
@@ -35,9 +35,6 @@
     <t>date de facture</t>
   </si>
   <si>
-    <t>destinatire client</t>
-  </si>
-  <si>
     <t>etat de facture</t>
   </si>
   <si>
@@ -72,6 +69,12 @@
   </si>
   <si>
     <t>si &gt; 500€</t>
+  </si>
+  <si>
+    <t>SOMME DES LIGNES</t>
+  </si>
+  <si>
+    <t>destinataire client</t>
   </si>
 </sst>
 </file>
@@ -81,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +128,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -140,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -148,29 +158,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color auto="1"/>
+      </right>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G5"/>
+  <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,87 +554,101 @@
     <col min="8" max="8" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6">
+        <v>100000</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8">
-        <v>100000</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="6">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>25569</v>
       </c>
       <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="5" customFormat="1" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11">
+        <f>SUM(G5:G5)</f>
         <v>99.99</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B2:G2"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>